<commit_message>
Dinamica de maquina agregada
Ecuaciones de Eq' y Ed' agregadas
La integracion funciona.
</commit_message>
<xml_diff>
--- a/BUSDATA_fallabarra.xlsx
+++ b/BUSDATA_fallabarra.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Google Drive\Conversión y Transporte de Energía\CT4211 - Potencia III\SepDic2017 - Prof. Bermudez\Programas\Estabilidad-Transitoria-PIII\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11610" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="NODOS" sheetId="1" r:id="rId1"/>
-    <sheet name="RAMAS PRE" sheetId="2" r:id="rId2"/>
-    <sheet name="RAMA FALLA" sheetId="7" r:id="rId3"/>
-    <sheet name="RAMAS POST" sheetId="8" r:id="rId4"/>
-    <sheet name="GENERADORES" sheetId="3" r:id="rId5"/>
-    <sheet name="FALLAS" sheetId="10" r:id="rId6"/>
-    <sheet name="INTEGRACION" sheetId="9" r:id="rId7"/>
+    <sheet name="NODOS_FALLA" sheetId="11" r:id="rId2"/>
+    <sheet name="RAMAS PRE" sheetId="2" r:id="rId3"/>
+    <sheet name="RAMA FALLA" sheetId="7" r:id="rId4"/>
+    <sheet name="RAMAS POST" sheetId="8" r:id="rId5"/>
+    <sheet name="GENERADORES" sheetId="3" r:id="rId6"/>
+    <sheet name="FALLAS" sheetId="10" r:id="rId7"/>
+    <sheet name="INTEGRACION" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
   <si>
     <t>BARRA</t>
   </si>
@@ -96,18 +102,6 @@
     <t>TAP</t>
   </si>
   <si>
-    <t>RESISTENCIA ITNERNA</t>
-  </si>
-  <si>
-    <t>REACTANCIA TRANSITORIA</t>
-  </si>
-  <si>
-    <t>TENSION INTERNA</t>
-  </si>
-  <si>
-    <t>ANGULO d0</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
@@ -162,20 +156,44 @@
     <t>Xqpp</t>
   </si>
   <si>
-    <t>Tq0p</t>
-  </si>
-  <si>
-    <t>Td0p</t>
+    <t>tdop</t>
+  </si>
+  <si>
+    <t>tqop</t>
+  </si>
+  <si>
+    <t>tdopp</t>
+  </si>
+  <si>
+    <t>tqopp</t>
+  </si>
+  <si>
+    <t>Kv</t>
+  </si>
+  <si>
+    <t>Kt</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Tv</t>
+  </si>
+  <si>
+    <t>Tt</t>
+  </si>
+  <si>
+    <t>Devanado Campo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +219,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -247,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -283,11 +307,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -322,9 +370,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -335,7 +380,19 @@
     <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -610,7 +667,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -847,209 +904,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H5"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G2" s="2">
-        <f>F2/2</f>
-        <v>0.05</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="G3" s="2">
-        <f t="shared" ref="G3:G5" si="0">F3/2</f>
-        <v>0.1</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="7">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7">
-        <v>3</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0.03</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="H4" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>-1.5</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="2"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1081,7 +944,7 @@
         <v>13</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>22</v>
@@ -1204,7 +1067,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1216,7 +1079,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="15"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1228,7 +1091,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="15"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1240,7 +1103,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="15"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1252,12 +1115,12 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1289,7 +1152,7 @@
         <v>13</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>22</v>
@@ -1412,7 +1275,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="15"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1424,7 +1287,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="15"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1436,7 +1299,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="15"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1448,7 +1311,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="15"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1460,7 +1323,215 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" s="2">
+        <f>F2/2</f>
+        <v>0.05</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G5" si="0">F3/2</f>
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>-1.5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="2"/>
     </row>
   </sheetData>
@@ -1468,158 +1539,196 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="23" t="s">
+      <c r="N1" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="O1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q1" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="10">
-        <v>0</v>
-      </c>
-      <c r="C2" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="D2" s="10">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="10">
-        <v>0</v>
-      </c>
-      <c r="F2" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="G2" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="H2" s="10">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="I2" s="10">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="J2" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="K2" s="10">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="L2" s="10">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M2" s="10">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="N2" s="10">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="O2" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="23">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C2" s="23">
+        <v>1.3129999999999999</v>
+      </c>
+      <c r="D2" s="23">
+        <v>0.18</v>
+      </c>
+      <c r="E2" s="23">
+        <v>0.156</v>
+      </c>
+      <c r="F2" s="23">
+        <v>1.258</v>
+      </c>
+      <c r="G2" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="H2" s="23">
+        <v>0.156</v>
+      </c>
+      <c r="I2" s="24">
+        <v>1E+100</v>
+      </c>
+      <c r="J2" s="24">
+        <v>1E+100</v>
+      </c>
+      <c r="K2" s="23">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="L2" s="23">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="M2" s="23">
+        <v>1.51</v>
+      </c>
+      <c r="N2" s="23">
+        <v>1</v>
+      </c>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="25">
+        <v>2.4</v>
+      </c>
+      <c r="R2" s="24">
+        <v>10000000000</v>
+      </c>
+      <c r="S2" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="T2" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="10">
-        <v>0</v>
-      </c>
-      <c r="C3" s="10">
+      <c r="B3" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="D3" s="23">
         <v>0.12</v>
       </c>
-      <c r="D3" s="10">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="10">
-        <v>0</v>
-      </c>
-      <c r="F3" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="G3" s="10">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="H3" s="10">
-        <v>2.15</v>
-      </c>
-      <c r="I3" s="10">
-        <v>2.23</v>
-      </c>
-      <c r="J3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="K3" s="10">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="L3" s="10">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M3" s="10">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="N3" s="10">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="O3" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E3" s="23">
+        <v>0.104</v>
+      </c>
+      <c r="F3" s="23">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="G3" s="23">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="H3" s="23">
+        <v>0.104</v>
+      </c>
+      <c r="I3" s="24">
+        <v>1E+100</v>
+      </c>
+      <c r="J3" s="24">
+        <v>1E+100</v>
+      </c>
+      <c r="K3" s="23">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="L3" s="23">
+        <v>9.4500000000000001E-2</v>
+      </c>
+      <c r="M3" s="23">
+        <v>3.3980000000000001</v>
+      </c>
+      <c r="N3" s="23">
+        <v>1</v>
+      </c>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="25">
+        <v>2.4</v>
+      </c>
+      <c r="R3" s="24">
+        <v>10000000000</v>
+      </c>
+      <c r="S3" s="23">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -1636,91 +1745,91 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>36</v>
+      <c r="A1" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
-        <v>0</v>
-      </c>
-      <c r="B2" s="21">
+      <c r="A2" s="20">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20">
         <v>3</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="21">
         <v>3</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1728,7 +1837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1743,7 +1852,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B1" s="13">
         <v>60</v>
@@ -1751,7 +1860,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B2" s="13">
         <v>4</v>
@@ -1759,7 +1868,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B3" s="13">
         <v>10</v>
@@ -1767,7 +1876,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B4" s="13">
         <v>250</v>
@@ -1775,7 +1884,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B5" s="13">
         <v>0.5</v>

</xml_diff>